<commit_message>
Kopieren der Spalte aus Primärexcel funktioniert
</commit_message>
<xml_diff>
--- a/VorlageTabsam.xlsx
+++ b/VorlageTabsam.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Napfgasse 6, 8022 Zürich
 Telefon 044 412 08 00
@@ -48,7 +48,40 @@
     <t>Erstellt am: 28.04.2022</t>
   </si>
   <si>
-    <t>Zusammenfassung Siedlungsberichte Mehr als Wohnen</t>
+    <t>Mehr als Wohnen</t>
+  </si>
+  <si>
+    <t>              </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Quelle: Statistik Stadt Zürich</t>
+  </si>
+  <si>
+    <t>Vergleich Siedlungsauswertungen T_2.1-2.6, G_3.2, T_3.4-3.11, T_3.13-3.15, T_5.1-5.3</t>
+  </si>
+  <si>
+    <t>Vergleich Siedlungsauswertung x.x</t>
+  </si>
+  <si>
+    <t>T_2</t>
+  </si>
+  <si>
+    <t>T_3</t>
+  </si>
+  <si>
+    <t>T_4</t>
+  </si>
+  <si>
+    <t>T_5</t>
+  </si>
+  <si>
+    <t>Vergleich Siedlungsauswertung T_4.7</t>
+  </si>
+  <si>
+    <t>Vergleich Siedlungsauswertung T_4.14</t>
   </si>
 </sst>
 </file>
@@ -58,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#\ ###\ ##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +138,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -133,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -181,11 +233,20 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -538,10 +599,10 @@
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
@@ -616,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
@@ -626,8 +687,12 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="C11" s="17"/>
       <c r="D11" s="20"/>
       <c r="E11" s="19"/>
@@ -636,8 +701,12 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="C12" s="17"/>
       <c r="D12" s="20"/>
       <c r="E12" s="19"/>
@@ -646,8 +715,12 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="C13" s="17"/>
       <c r="D13" s="20"/>
       <c r="E13" s="19"/>
@@ -656,8 +729,12 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="C14" s="17"/>
       <c r="D14" s="20"/>
       <c r="E14" s="19"/>
@@ -1408,15 +1485,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="11" style="22"/>
+    <col min="1" max="16384" width="11" style="21"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="23"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>